<commit_message>
include MPS accel, improve efficiency of feature measurement
</commit_message>
<xml_diff>
--- a/analyze/demo/fname_resolution_location_eye.xlsx
+++ b/analyze/demo/fname_resolution_location_eye.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1522100\Documents\PhD Work\Python Scripts\Github\SLOctolyzer\analyze\demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s1522100/Documents/SLOctolyzer/analyze/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE47807-1B70-4657-8A6A-DB897A463DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C376DB80-661E-8F44-829A-AF2124462427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5980" yWindow="4420" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fname_resolution_location_eye" sheetId="1" r:id="rId1"/>
@@ -636,17 +636,17 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="19" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -660,7 +660,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -674,7 +674,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -702,12 +702,12 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -715,7 +715,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -723,7 +723,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -737,7 +737,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -751,7 +751,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>

</xml_diff>